<commit_message>
till add to cart
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/testdata.xlsx
+++ b/src/main/java/testdata/testdata.xlsx
@@ -5,14 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\om sai ram\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\om sai ram\Desktop\E2EProject\src\main\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Regdata" sheetId="2" r:id="rId1"/>
+    <sheet name="Searchdata" sheetId="3" r:id="rId2"/>
+    <sheet name="wishlistdata" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
   <si>
     <t>password</t>
   </si>
@@ -71,13 +73,97 @@
     <t>zx@gmail.com</t>
   </si>
   <si>
-    <t>zx1@yahoo.com</t>
-  </si>
-  <si>
-    <t>as1@yahoo.com</t>
-  </si>
-  <si>
-    <t>qw1@yahoo.com</t>
+    <t>Macbook</t>
+  </si>
+  <si>
+    <t>Searchtext</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>iPhone</t>
+  </si>
+  <si>
+    <t>searchuname</t>
+  </si>
+  <si>
+    <t>searchpwd</t>
+  </si>
+  <si>
+    <t>vsl@gmail.com</t>
+  </si>
+  <si>
+    <t>Lp@absms4</t>
+  </si>
+  <si>
+    <t>Apple Cinema 30</t>
+  </si>
+  <si>
+    <t>iMac</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Product 8</t>
+  </si>
+  <si>
+    <t>Pro</t>
+  </si>
+  <si>
+    <t>Palm Treo Pro</t>
+  </si>
+  <si>
+    <t>MacBook Pro</t>
+  </si>
+  <si>
+    <t>MacBook Air</t>
+  </si>
+  <si>
+    <t>Mac</t>
+  </si>
+  <si>
+    <t>Productname</t>
+  </si>
+  <si>
+    <t>wishproduct</t>
+  </si>
+  <si>
+    <t>vs@yahoo.com</t>
+  </si>
+  <si>
+    <t>sl@gmail.com</t>
+  </si>
+  <si>
+    <t>vsl@hotmail.com</t>
+  </si>
+  <si>
+    <t>Addtocartfromwishlist</t>
+  </si>
+  <si>
+    <t>Removefromwishlist</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Apple Cinema 30"</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>HTC Touch HD</t>
   </si>
 </sst>
 </file>
@@ -107,7 +193,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,6 +212,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -140,12 +238,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -429,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +574,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D2">
         <v>1234556789</v>
@@ -491,7 +594,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D3">
         <v>9876543210</v>
@@ -511,7 +614,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D4">
         <v>6789102345</v>
@@ -538,4 +641,277 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId10"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1" display="http://tutorialsninja.com/demo/index.php?route=product/product&amp;product_id=44&amp;search=macbook"/>
+    <hyperlink ref="D8" r:id="rId2" display="http://tutorialsninja.com/demo/index.php?route=product/product&amp;product_id=41&amp;search=mac"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="http://tutorialsninja.com/demo/index.php?route=product/product&amp;product_id=28&amp;search=h"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>